<commit_message>
add sd card and adc test
</commit_message>
<xml_diff>
--- a/EmbedFire_STM32H750XB/STM32H750X_CORE_引脚分布.xlsx
+++ b/EmbedFire_STM32H750XB/STM32H750X_CORE_引脚分布.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\3.git\1.Github\ThreadX_H750\EmbedFire_STM32H750XB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC05356-0457-4DFE-84F6-B230DFE8B999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671AFBC5-27C0-4E58-BA3C-E9802C0D0305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="核心板" sheetId="1" r:id="rId1"/>
+    <sheet name="底板" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="280">
   <si>
     <t>PB8</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -941,6 +942,104 @@
   <si>
     <t>KEY
 默认外部下拉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SDIO_D2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SDIO_D3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SDIO_CMD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SDIO_CLK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SDIO_D0</t>
+  </si>
+  <si>
+    <t>SDIO_D1</t>
+  </si>
+  <si>
+    <t>PC8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC10</t>
+  </si>
+  <si>
+    <t>PC11</t>
+  </si>
+  <si>
+    <t>PD2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED_R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED_G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED_B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SD Card
+需要拉低PC2，不能和WIFI模块共用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WIFI
+不能和SD Card模块共用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PI11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL_REG_ON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL_HOST_WAKE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1539,7 +1638,7 @@
   <dimension ref="A1:Q45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="A3:C5"/>
+      <selection sqref="A1:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2618,4 +2717,224 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45FDD07-1E4B-4583-85A5-5B5A16038384}">
+  <dimension ref="A1:F36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>274</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="34"/>
+      <c r="B2" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="34"/>
+      <c r="B3" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="34"/>
+      <c r="B4" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="34"/>
+      <c r="B5" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="27"/>
+      <c r="B6" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>265</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="20"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="27"/>
+      <c r="B12" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="22"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="22"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="22"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="22"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A19" s="27"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="22"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="22"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="27"/>
+      <c r="B23" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="36" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A6"/>
+    <mergeCell ref="A7:A14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A21:A23"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>